<commit_message>
ARomao - Exportar para EXCEL - 20/07/2018
</commit_message>
<xml_diff>
--- a/Hydra.Such.Portal/Hydra.Such.Portal/wwwroot/Upload/temp/ARomao_such_pt.xlsx
+++ b/Hydra.Such.Portal/Hydra.Such.Portal/wwwroot/Upload/temp/ARomao_such_pt.xlsx
@@ -6,51 +6,48 @@
     <workbookView tabRatio="600"/>
   </bookViews>
   <sheets>
-    <sheet name="Pedidos de Aquisição" sheetId="1" r:id="rId3"/>
+    <sheet name="Telemóveis Cartões" sheetId="1" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
-  <si>
-    <t xml:space="preserve">Nº</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+  <si>
+    <t xml:space="preserve">Nº Cartão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo Serviço</t>
   </si>
   <si>
     <t xml:space="preserve">Estado</t>
   </si>
   <si>
-    <t xml:space="preserve">Nome Processo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestor Processo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valor Preço Base</t>
+    <t xml:space="preserve">Conta SUCH</t>
   </si>
   <si>
     <t xml:space="preserve">Código Região</t>
   </si>
   <si>
-    <t xml:space="preserve">Codigo Área Funcional</t>
+    <t xml:space="preserve">Código Área Funcional</t>
   </si>
   <si>
     <t xml:space="preserve">Código Centro Responsabilidade</t>
   </si>
   <si>
-    <t xml:space="preserve">PS00001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teste nunorato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12</t>
+    <t xml:space="preserve">111111111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Por Activar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123123123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
   </si>
   <si>
     <t xml:space="preserve">32</t>
@@ -59,13 +56,25 @@
     <t xml:space="preserve">018SI</t>
   </si>
   <si>
-    <t xml:space="preserve">PS00002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PS00004</t>
+    <t xml:space="preserve">456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7777777777</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">969999999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1338340476</t>
   </si>
 </sst>
 </file>
@@ -137,21 +146,20 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2"/>
       <c r="E2" t="s">
         <v>11</v>
       </c>
@@ -161,37 +169,52 @@
       <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>